<commit_message>
Edited documentation and graphs
</commit_message>
<xml_diff>
--- a/outputfiles/Metrics/Graphs/LinesOfCode.xlsx
+++ b/outputfiles/Metrics/Graphs/LinesOfCode.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\University\uol-inf co7506\Git\Assignment3\CodeAnalysisToolkit\outputfiles\Charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\University\uol-inf co7506\Git\Assignment3\CodeAnalysisToolkit\outputfiles\Metrics\Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="LinesOfCode" sheetId="1" r:id="rId1"/>
@@ -6937,11 +6937,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="395285088"/>
-        <c:axId val="395286656"/>
+        <c:axId val="340628048"/>
+        <c:axId val="340628440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="395285088"/>
+        <c:axId val="340628048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6984,7 +6984,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395286656"/>
+        <c:crossAx val="340628440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6992,7 +6992,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="395286656"/>
+        <c:axId val="340628440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7043,7 +7043,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395285088"/>
+        <c:crossAx val="340628048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7935,11 +7935,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B697"/>
   <sheetViews>
-    <sheetView topLeftCell="A659" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -13527,7 +13529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X73" sqref="X73"/>
     </sheetView>
   </sheetViews>

</xml_diff>